<commit_message>
fake data now 100,000
</commit_message>
<xml_diff>
--- a/DDGwork.xlsx
+++ b/DDGwork.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="26">
   <si>
     <t>Year</t>
   </si>
@@ -90,9 +90,6 @@
     <t>remove sex strat from infant/neonatal deahts</t>
   </si>
   <si>
-    <t>Current</t>
-  </si>
-  <si>
     <t>Supress N &lt; 12</t>
   </si>
   <si>
@@ -100,6 +97,12 @@
   </si>
   <si>
     <t xml:space="preserve">No sex; </t>
+  </si>
+  <si>
+    <t>No Supression</t>
+  </si>
+  <si>
+    <t>no sex age &lt; 1</t>
   </si>
 </sst>
 </file>
@@ -309,7 +312,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -436,122 +439,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -884,7 +780,7 @@
   <dimension ref="B3:R23"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -900,17 +796,22 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" t="s">
         <v>21</v>
       </c>
-      <c r="G3" t="s">
+      <c r="J3" t="s">
         <v>22</v>
       </c>
-      <c r="J3" t="s">
+      <c r="M3" t="s">
         <v>23</v>
       </c>
-      <c r="M3" t="s">
-        <v>24</v>
+    </row>
+    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -1404,51 +1305,51 @@
       </c>
       <c r="C22" s="23"/>
       <c r="D22" s="24">
-        <f>SUM(D8:D17)</f>
+        <f t="shared" ref="D22:O22" si="0">SUM(D8:D17)</f>
         <v>13</v>
       </c>
       <c r="E22" s="25">
-        <f>SUM(E8:E17)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="F22" s="26">
-        <f>SUM(F8:F17)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="G22" s="24">
-        <f>SUM(G8:G17)</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="H22" s="25">
-        <f>SUM(H8:H17)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="I22" s="26">
-        <f>SUM(I8:I17)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="J22" s="25">
-        <f>SUM(J8:J17)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="K22" s="25">
-        <f>SUM(K8:K17)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="L22" s="26">
-        <f>SUM(L8:L17)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="M22" s="24">
-        <f>SUM(M8:M17)</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="N22" s="25">
-        <f>SUM(N8:N17)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="O22" s="26">
-        <f>SUM(O8:O17)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
@@ -1458,39 +1359,39 @@
       </c>
       <c r="C23" s="28"/>
       <c r="D23" s="29">
-        <f>SUM(D8:D20)</f>
+        <f t="shared" ref="D23:J23" si="1">SUM(D8:D20)</f>
         <v>20</v>
       </c>
       <c r="E23" s="30">
-        <f>SUM(E8:E20)</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="F23" s="31">
-        <f>SUM(F8:F20)</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="G23" s="29">
-        <f>SUM(G8:G20)</f>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="H23" s="30">
-        <f>SUM(H8:H20)</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="I23" s="31">
-        <f>SUM(I8:I20)</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="J23" s="30">
-        <f>SUM(J8:J20)</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="K23" s="30">
-        <f t="shared" ref="K23:L23" si="0">SUM(K8:K20)</f>
+        <f t="shared" ref="K23:L23" si="2">SUM(K8:K20)</f>
         <v>7</v>
       </c>
       <c r="L23" s="31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="M23" s="29">
@@ -1526,7 +1427,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>